<commit_message>
further mdx query testing
</commit_message>
<xml_diff>
--- a/query.xlsx
+++ b/query.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\Studia\data_warehouse\Schemas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub Machura\source\repos\Machmurka\DataWarehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E08D7D84-01C4-4FE3-A495-9E7681FC5012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637942BE-C47C-4D6C-B340-AE21059BAF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="33068" windowHeight="17948" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="num_ticket by category" sheetId="1" r:id="rId1"/>
@@ -26,23 +26,23 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId11"/>
-    <pivotCache cacheId="35" r:id="rId12"/>
-    <pivotCache cacheId="119" r:id="rId13"/>
-    <pivotCache cacheId="140" r:id="rId14"/>
-    <pivotCache cacheId="162" r:id="rId15"/>
-    <pivotCache cacheId="187" r:id="rId16"/>
-    <pivotCache cacheId="202" r:id="rId17"/>
-    <pivotCache cacheId="229" r:id="rId18"/>
-    <pivotCache cacheId="244" r:id="rId19"/>
-    <pivotCache cacheId="257" r:id="rId20"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
+    <pivotCache cacheId="3" r:id="rId14"/>
+    <pivotCache cacheId="4" r:id="rId15"/>
+    <pivotCache cacheId="5" r:id="rId16"/>
+    <pivotCache cacheId="6" r:id="rId17"/>
+    <pivotCache cacheId="7" r:id="rId18"/>
+    <pivotCache cacheId="8" r:id="rId19"/>
+    <pivotCache cacheId="9" r:id="rId20"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\Marcel\AppData\Local\Temp\tmp95E4.odc" keepAlive="1" name="localhost call_masterDW_new" type="5" refreshedVersion="8" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" odcFile="C:\Users\Marcel\AppData\Local\Temp\tmp95E4.odc" keepAlive="1" name="localhost call_masterDW_new" type="5" refreshedVersion="8" background="1">
     <dbPr connection="Provider=MSOLAP.8;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=call_masterDW_new;Data Source=localhost;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error;Update Isolation Level=2" command="Call Master DW" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
   </connection>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="87">
   <si>
     <t>Column Labels</t>
   </si>
@@ -131,12 +131,192 @@
   </si>
   <si>
     <t>Reunion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Measures].[avg_resolution_time]} ON COLUMNS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Dim Date].[Creation Month].Members} ON ROWS</t>
+  </si>
+  <si>
+    <t>FROM [Call Master DW];</t>
+  </si>
+  <si>
+    <t>MDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WITH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  MEMBER [Prev month amount] AS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ([Measures].[number_tickets], PARALLELPERIOD([Dim Date].[Hierarchy].[Creation Month], 1,[Dim Date].[Hierarchy].CurrentMember))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Measures].[number_tickets], [Prev month amount]} ON COLUMNS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NON EMPTY EXCEPT([Dim Category].[Name].Members, {[Dim Category].[Name].[All], [Dim Category].[Name].[UNKNOWNMEMBER]}) ON ROWS</t>
+  </si>
+  <si>
+    <t>FROM [Call Master DW]</t>
+  </si>
+  <si>
+    <t>WHERE (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  [Dim Date].[Hierarchy].[Creation Year].[2023].[May]</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SET [NonEmptyEmployees] AS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    EXCEPT(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      [Dim Employees].[Name].Members, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      {[Dim Employees].[Name].[]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SET [TopPerformingAgents] AS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    TOPCOUNT(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      [NonEmptyEmployees], </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      [Measures].[number_tickets]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Measures].[number_tickets]} ON COLUMNS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NON EMPTY {[Dim Date].[Creation Month].Members * [TopPerformingAgents]} ON ROWS</t>
+  </si>
+  <si>
+    <t>Komentarz:</t>
+  </si>
+  <si>
+    <t>nula wyrzuca na month/emplyees coś zjebane z insertami albo brak mojej umiejętności w mdx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SET [NonEmptyDepartments] AS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      [Dim Department].[Name].Members, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      {[Dim Department].[Name].[(null)], [Dim Department].[Name].[Unknown]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Dim Date].[Hierarchy].[Creation Year].Members, [Dim Date].[Hierarchy].[Creation Month].Members} * [NonEmptyDepartments] ON ROWS</t>
+  </si>
+  <si>
+    <t>komentarz:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wywala (null) i (unknow) w datach tak o </t>
+  </si>
+  <si>
+    <t>SET [NonEmptyNames] AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Except(</t>
+  </si>
+  <si>
+    <t>[Dim Category].[Name].Members, {[Dim Category].[Name].[null]}</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SET [TopResolvedIssues] AS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [NonEmptyNames], </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[TopResolvedIssues]} ON ROWS</t>
+  </si>
+  <si>
+    <t>mimo exclude (null) nadal go pokazuje w name</t>
+  </si>
+  <si>
+    <t>WITH</t>
+  </si>
+  <si>
+    <t>SET [NonEmptySt] AS</t>
+  </si>
+  <si>
+    <t>Except ([Dim Feedback].[Satisfaction Level].Members,{[Dim Feedback].[Satisfaction Level].[All].UNKNOWNMEMBER})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Measures].[avg_response_time]} ON COLUMNS,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[NonEmptySt]} ON ROWS</t>
+  </si>
+  <si>
+    <t>avg response time wyświetla się jako "0,00321"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pojawia się (null) jako jedna z nazw </t>
+  </si>
+  <si>
+    <t>Except ([Dim Feedback].[Satisfaction Level].Members,{[Dim Feedback].[Satisfaction Level].[All].UNKNOWNMEMBER,[Dim Feedback].[Satisfaction Level].[(null)]})</t>
+  </si>
+  <si>
+    <t>SET [NonEmptyCat] AS</t>
+  </si>
+  <si>
+    <t>Except ([Dim Category].[Name].Members,{[Dim Category].[Name].[All].UNKNOWNMEMBE})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[NonEmptySt] * [NonEmptyCat]} ON ROWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">komentarz: </t>
+  </si>
+  <si>
+    <t>mimo exception wywala (null) w SatScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Dim Feedback].[Satisfaction Level].Members *[Dim Feedback].[Customer Location].Members} ON ROWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ten sam problem z NULL dla Satisfacion level </t>
+  </si>
+  <si>
+    <t>SET [NonEmptyDEP] AS</t>
+  </si>
+  <si>
+    <t>Except ([Dim Department].[Name].Members,{[Dim Department].[Name].[All].UNKNOWNMEMBE})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  {[Dim Date].[Hierarchy].[Creation Month]*[NonEmptySt] * [NonEmptyDEP]} ON ROWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Komentarz: to samo co wcześniej z NULL, Dodany podział na date </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,60 +794,59 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — akcent 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — akcent 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — akcent 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akcent 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akcent 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akcent 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akcent 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akcent 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akcent 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Dane wejściowe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Dane wyjściowe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Dobry" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Komórka połączona" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Komórka zaznaczona" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Nagłówek 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutralny" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Obliczenia" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Suma" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Tekst objaśnienia" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Tekst ostrzeżenia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Tytuł" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Uwaga" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Zły" xfId="7" builtinId="27" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -683,7 +862,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.914456134262" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.914456134262" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF0D000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Category].[Name].[Name]" caption="Name" numFmtId="0" hierarchy="1" level="1">
@@ -806,7 +985,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.964038773149" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.964038773149" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01010000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Measures].[number_tickets]" caption="number_tickets" numFmtId="0" hierarchy="34" level="32767"/>
@@ -914,7 +1093,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.94385127315" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.94385127315" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF23000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Category].[Name].[Name]" caption="Name" numFmtId="0" hierarchy="1" level="1">
@@ -1037,7 +1216,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.949097916666" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.949097916666" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF77000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Measures].[avrage_resolutionTime]" caption="avrage_resolutionTime" numFmtId="0" hierarchy="35" level="32767"/>
@@ -1148,7 +1327,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.951331365737" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.951331365737" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF8C000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="10">
     <cacheField name="[Date].[Creation Month].[Creation Month]" caption="Creation Month" numFmtId="0" hierarchy="7" level="1" mappingCount="2">
@@ -1315,7 +1494,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.955792939814" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.955792939814" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFFA2000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
     <cacheField name="[Measures].[number_tickets]" caption="number_tickets" numFmtId="0" hierarchy="34" level="32767"/>
@@ -1438,7 +1617,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.957646990741" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.957646990741" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFFBB000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[Feedback].[Satisfaction Level].[Satisfaction Level]" caption="Satisfaction Level" numFmtId="0" hierarchy="22" level="1">
@@ -1534,7 +1713,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.96056446759" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.96056446759" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFFCA000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[Measures].[avrage_resolutionTime]" caption="avrage_resolutionTime" numFmtId="0" hierarchy="35" level="32767"/>
@@ -1630,7 +1809,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.961701851855" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.961701851855" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFFE5000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Category].[Name].[Name]" caption="Name" numFmtId="0" hierarchy="1" level="1">
@@ -1738,7 +1917,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.963350347221" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Marcel Kowalik" refreshedDate="45399.963350347221" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFFF4000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Measures].[number_tickets]" caption="number_tickets" numFmtId="0" hierarchy="34" level="32767"/>
@@ -1846,7 +2025,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -1967,7 +2146,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="257" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0900-000009000000}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2081,7 +2260,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -2202,7 +2381,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="119" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2299,7 +2478,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="140" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisCol" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -2449,7 +2628,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="162" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000004000000}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2570,7 +2749,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="187" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000005000000}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -2660,7 +2839,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="202" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000006000000}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2750,7 +2929,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="229" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0700-000007000000}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -2864,7 +3043,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="244" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000008000000}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:E6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -2978,9 +3157,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3018,7 +3197,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3124,7 +3303,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3266,28 +3445,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3295,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3312,60 +3493,104 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3374,20 +3599,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3395,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3412,60 +3637,102 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3474,21 +3741,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3496,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3513,60 +3782,135 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3575,31 +3919,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -3613,21 +3957,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3636,23 +4005,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3660,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3677,112 +4048,181 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3790,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3807,60 +4247,110 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3869,26 +4359,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -3902,50 +4392,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -3959,21 +4491,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3982,20 +4555,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="5" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4003,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4020,83 +4595,129 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4104,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4121,60 +4742,80 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" t="s">
+        <v>79</v>
+      </c>
+      <c r="N12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>